<commit_message>
only allow selecting unlocked cells
</commit_message>
<xml_diff>
--- a/src/main/webapp/WEB-INF/book/Business Trip Request.xlsx
+++ b/src/main/webapp/WEB-INF/book/Business Trip Request.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10910"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hawk/Documents/workspace/KEIKAI-SPACE/tutorial/src/main/webapp/WEB-INF/book/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{913F9CA1-1B6E-8E4E-8D82-FB5D9AD5A60F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="460" windowWidth="33600" windowHeight="20460" tabRatio="500"/>
+    <workbookView xWindow="560" yWindow="2000" windowWidth="33600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leave" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
     <definedName name="arrangement">Sheet1!$A$1:$A$4</definedName>
     <definedName name="arrangment">Sheet1!$A$1:$A$4</definedName>
   </definedNames>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -93,7 +94,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -106,6 +107,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Helvetica"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -127,80 +129,96 @@
       <sz val="24"/>
       <color theme="0"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF1E474E"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="24"/>
       <color rgb="FF1E474E"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="0"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="0"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
       <color rgb="FF1E474E"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="0"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="20"/>
       <color theme="0"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1" tint="0.249977111117893"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="2" tint="-0.249977111117893"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
       <color rgb="FF1E474E"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
       <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="9">
@@ -349,13 +367,6 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -366,10 +377,6 @@
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="14" fontId="16" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -378,6 +385,20 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -399,23 +420,17 @@
     <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="17" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -437,6 +452,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -482,6 +500,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1025"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -513,9 +534,7 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Helvetica"/>
-                  <a:ea typeface="Helvetica"/>
-                  <a:cs typeface="Helvetica"/>
+                  <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Submit</a:t>
               </a:r>
@@ -549,6 +568,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -580,9 +602,7 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Helvetica"/>
-                  <a:ea typeface="Helvetica"/>
-                  <a:cs typeface="Helvetica"/>
+                  <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Cancel</a:t>
               </a:r>
@@ -616,6 +636,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -647,9 +670,7 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Helvetica"/>
-                  <a:ea typeface="Helvetica"/>
-                  <a:cs typeface="Helvetica"/>
+                  <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Approve</a:t>
               </a:r>
@@ -683,6 +704,9 @@
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
+                </a:ext>
               </a:extLst>
             </xdr:cNvPr>
             <xdr:cNvSpPr/>
@@ -714,9 +738,7 @@
                   <a:solidFill>
                     <a:srgbClr val="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="Helvetica"/>
-                  <a:ea typeface="Helvetica"/>
-                  <a:cs typeface="Helvetica"/>
+                  <a:latin typeface="Helvetica" pitchFamily="2" charset="0"/>
                 </a:rPr>
                 <a:t>Reject</a:t>
               </a:r>
@@ -993,7 +1015,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M27"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
@@ -1029,12 +1051,12 @@
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
@@ -1056,14 +1078,14 @@
     </row>
     <row r="4" spans="2:13" ht="23" x14ac:dyDescent="0.2">
       <c r="B4" s="4"/>
-      <c r="C4" s="33" t="s">
+      <c r="C4" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
       <c r="G4" s="6"/>
       <c r="H4" s="13" t="s">
         <v>6</v>
@@ -1071,7 +1093,7 @@
       <c r="I4" s="14"/>
       <c r="J4" s="17">
         <f ca="1">TODAY()</f>
-        <v>43385</v>
+        <v>43389</v>
       </c>
       <c r="K4" s="7"/>
       <c r="L4" s="7"/>
@@ -1079,7 +1101,7 @@
     </row>
     <row r="5" spans="2:13" ht="10" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="4"/>
-      <c r="C5" s="33"/>
+      <c r="C5" s="30"/>
       <c r="D5" s="19"/>
       <c r="E5" s="19"/>
       <c r="F5" s="19"/>
@@ -1093,12 +1115,12 @@
     </row>
     <row r="6" spans="2:13" ht="23" x14ac:dyDescent="0.25">
       <c r="B6" s="4"/>
-      <c r="C6" s="33" t="s">
+      <c r="C6" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
+      <c r="F6" s="33"/>
       <c r="G6" s="9"/>
       <c r="H6" s="16" t="s">
         <v>7</v>
@@ -1106,19 +1128,19 @@
       <c r="I6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="32">
+      <c r="J6" s="29">
         <f ca="1">TODAY()</f>
-        <v>43385</v>
+        <v>43389</v>
       </c>
       <c r="K6" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="L6" s="32"/>
+      <c r="L6" s="29"/>
       <c r="M6" s="4"/>
     </row>
     <row r="7" spans="2:13" ht="10" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4"/>
-      <c r="C7" s="33"/>
+      <c r="C7" s="30"/>
       <c r="D7" s="20"/>
       <c r="E7" s="20"/>
       <c r="F7" s="21"/>
@@ -1132,12 +1154,12 @@
     </row>
     <row r="8" spans="2:13" ht="23" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
-      <c r="C8" s="33" t="s">
+      <c r="C8" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
       <c r="G8" s="7"/>
       <c r="H8" s="16" t="s">
         <v>8</v>
@@ -1181,34 +1203,34 @@
     </row>
     <row r="11" spans="2:13" ht="41" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="22"/>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37"/>
-      <c r="H11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
       <c r="I11" s="22"/>
-      <c r="J11" s="34" t="s">
+      <c r="J11" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
+      <c r="K11" s="35"/>
+      <c r="L11" s="35"/>
       <c r="M11" s="22"/>
     </row>
     <row r="12" spans="2:13" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="22"/>
-      <c r="C12" s="40"/>
-      <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
-      <c r="F12" s="37"/>
-      <c r="G12" s="37"/>
-      <c r="H12" s="37"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
       <c r="I12" s="22"/>
-      <c r="J12" s="38"/>
-      <c r="K12" s="38"/>
-      <c r="L12" s="38"/>
+      <c r="J12" s="39"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="39"/>
       <c r="M12" s="22"/>
     </row>
     <row r="13" spans="2:13" ht="13" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
@@ -1220,22 +1242,22 @@
       <c r="G13" s="24"/>
       <c r="H13" s="24"/>
       <c r="I13" s="22"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="26"/>
-      <c r="L13" s="26"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="42"/>
+      <c r="L13" s="42"/>
       <c r="M13" s="22"/>
     </row>
     <row r="14" spans="2:13" ht="39" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="22"/>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="44" t="s">
+      <c r="D14" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="44"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="31"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
       <c r="H14" s="22"/>
       <c r="I14" s="22"/>
       <c r="J14" s="22"/>
@@ -1245,11 +1267,11 @@
     </row>
     <row r="15" spans="2:13" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="22"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="43"/>
-      <c r="E15" s="43"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
+      <c r="C15" s="25"/>
+      <c r="D15" s="44"/>
+      <c r="E15" s="44"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
       <c r="H15" s="22"/>
       <c r="I15" s="22"/>
       <c r="J15" s="22"/>
@@ -1259,11 +1281,11 @@
     </row>
     <row r="16" spans="2:13" ht="64" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="22"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="43"/>
-      <c r="E16" s="43"/>
-      <c r="F16" s="43"/>
-      <c r="G16" s="43"/>
+      <c r="C16" s="28"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
       <c r="H16" s="22"/>
       <c r="I16" s="22"/>
       <c r="J16" s="22"/>
@@ -1274,31 +1296,31 @@
       </c>
     </row>
     <row r="27" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G27" s="29"/>
+      <c r="G27" s="27"/>
     </row>
   </sheetData>
-  <sheetProtection sheet="1" objects="1" scenarios="1" autoFilter="0"/>
+  <sheetProtection sheet="1" objects="1" scenarios="1" selectLockedCells="1" autoFilter="0"/>
   <mergeCells count="11">
+    <mergeCell ref="J11:L11"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D11:H12"/>
+    <mergeCell ref="J12:L12"/>
+    <mergeCell ref="F2:I2"/>
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D6:F6"/>
     <mergeCell ref="D16:G16"/>
     <mergeCell ref="D15:G15"/>
     <mergeCell ref="D14:E14"/>
-    <mergeCell ref="J11:L11"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D11:H12"/>
-    <mergeCell ref="J12:L12"/>
-    <mergeCell ref="F2:I2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C23">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C19:C23" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>$C$18</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C18" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"$C$18,$C$19,$C$20,$C$21,$C$22,$C$23"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:E14">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D14:E14" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>arrangement</formula1>
     </dataValidation>
   </dataValidations>
@@ -1330,7 +1352,6 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -1353,7 +1374,6 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -1376,7 +1396,6 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
@@ -1399,29 +1418,15 @@
               </controlPr>
             </control>
           </mc:Choice>
-          <mc:Fallback/>
         </mc:AlternateContent>
       </controls>
     </mc:Choice>
-    <mc:Fallback/>
   </mc:AlternateContent>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Sheet1!$A$1:$A$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>F14:G14</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>